<commit_message>
Added new data, reviewed code
</commit_message>
<xml_diff>
--- a/Guide to BioCode Table.xlsx
+++ b/Guide to BioCode Table.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jandersen/Documents/Lab/BioCode/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\Dropbox\FA17\mlab\DNA-Sequencing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-27620" yWindow="7840" windowWidth="24960" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="-27615" yWindow="7845" windowWidth="24960" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -542,6 +539,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -812,16 +812,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -832,7 +832,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -843,7 +843,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -854,7 +854,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -865,7 +865,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -876,7 +876,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -887,7 +887,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -898,7 +898,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -909,7 +909,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -920,7 +920,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -931,7 +931,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -942,7 +942,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -953,7 +953,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -964,7 +964,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -975,7 +975,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -986,7 +986,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -997,7 +997,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>

</xml_diff>